<commit_message>
Jakbyś mógł to zamień skalę w tych wykresach z liniowej na logarytmiczną :) , i możesz zerknąć czy czegoś nie brakuje
</commit_message>
<xml_diff>
--- a/Pomiary_lab2.xlsx
+++ b/Pomiary_lab2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>f [ Hz ]</t>
   </si>
@@ -30,23 +30,41 @@
     <t>Vwy p-p / Vwe p-p</t>
   </si>
   <si>
-    <t>17m</t>
+    <t>t[us]</t>
   </si>
   <si>
-    <t>480u</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>580n</t>
+    <r>
+      <t>Faza [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Czcionka tekstu podstawowego"/>
+      </rPr>
+      <t>°</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>]</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +81,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Czcionka tekstu podstawowego"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -72,7 +111,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -95,36 +134,32 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -138,6 +173,29 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Charakterystyka</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> amplitudowo-częstotliwościowa </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -147,7 +205,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Arkusz1!$A$2:$A$19</c:f>
+              <c:f>Arkusz1!$A$3:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -210,9 +268,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$D$2:$D$19</c:f>
+              <c:f>Arkusz1!$D$3:$D$20</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1.2903225806451613E-3</c:v>
@@ -272,47 +330,357 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls/>
+        <c:hiLowLines/>
         <c:marker val="1"/>
-        <c:axId val="63722240"/>
-        <c:axId val="63723776"/>
+        <c:axId val="95093888"/>
+        <c:axId val="95095808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63722240"/>
+        <c:axId val="95093888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Częstotliwość</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> [Hz]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63723776"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95095808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63723776"/>
+        <c:axId val="95095808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Vwy/Vwe [V/V]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63722240"/>
+        <c:crossAx val="95093888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Charakterystyka</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> fazowa</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Arkusz1!$A$3:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$F$3:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>118.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110.88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95.04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>95.04</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>93.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>111.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>133.92000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>123.84</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>133.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-2.8799999999999955</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39.599999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls/>
+        <c:hiLowLines/>
+        <c:marker val="1"/>
+        <c:axId val="92532096"/>
+        <c:axId val="107285504"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="92532096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Częstotliwość</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> [Hz]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="107285504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="107285504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Faza [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL">
+                    <a:latin typeface="DaunPenh"/>
+                    <a:cs typeface="DaunPenh"/>
+                  </a:rPr>
+                  <a:t>°</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="92532096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -323,19 +691,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Wykres 2"/>
+        <xdr:cNvPr id="7" name="Wykres 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -345,6 +713,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Wykres 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -638,381 +1036,447 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A2:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:6" ht="15.75">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="4">
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="6">
         <v>12.4</v>
       </c>
-      <c r="C2">
+      <c r="C3" s="6">
         <f>16/1000</f>
         <v>1.6E-2</v>
       </c>
-      <c r="D2">
-        <f>C2/B2</f>
+      <c r="D3" s="7">
+        <f>C3/B3</f>
         <v>1.2903225806451613E-3</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="4">
+      <c r="E3" s="6">
+        <v>17000</v>
+      </c>
+      <c r="F3" s="6">
+        <f>180-((A3*360*E3)/1000000)</f>
+        <v>118.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3">
         <v>20</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="6">
         <v>16</v>
       </c>
-      <c r="C3">
+      <c r="C4" s="6">
         <v>0.14799999999999999</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D19" si="0">C3/B3</f>
+      <c r="D4" s="7">
+        <f t="shared" ref="D4:D20" si="0">C4/B4</f>
         <v>9.2499999999999995E-3</v>
       </c>
-      <c r="E3">
-        <v>9.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="4">
+      <c r="E4" s="6">
+        <v>9600</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" ref="F4:F20" si="1">180-((A4*360*E4)/1000000)</f>
+        <v>110.88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3">
         <v>50</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="6">
         <v>16.600000000000001</v>
       </c>
-      <c r="C4">
+      <c r="C5" s="6">
         <v>0.32</v>
       </c>
-      <c r="D4">
+      <c r="D5" s="7">
         <f t="shared" si="0"/>
         <v>1.9277108433734938E-2</v>
       </c>
-      <c r="E4">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="H4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="4">
+      <c r="E5" s="6">
+        <v>4600</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" si="1"/>
+        <v>97.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3">
         <v>100</v>
       </c>
-      <c r="B5">
+      <c r="B6" s="6">
         <v>16.600000000000001</v>
       </c>
-      <c r="C5">
+      <c r="C6" s="6">
         <v>0.63</v>
       </c>
-      <c r="D5">
+      <c r="D6" s="7">
         <f t="shared" si="0"/>
         <v>3.7951807228915661E-2</v>
       </c>
-      <c r="E5">
-        <v>2.36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="4">
+      <c r="E6" s="6">
+        <v>2360</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="1"/>
+        <v>95.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3">
         <v>200</v>
       </c>
-      <c r="B6">
+      <c r="B7" s="6">
         <v>16.600000000000001</v>
       </c>
-      <c r="C6">
+      <c r="C7" s="6">
         <v>1.24</v>
       </c>
-      <c r="D6">
+      <c r="D7" s="7">
         <f t="shared" si="0"/>
         <v>7.4698795180722879E-2</v>
       </c>
-      <c r="E6">
-        <v>1.18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="4">
+      <c r="E7" s="6">
+        <v>1180</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="1"/>
+        <v>95.04</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3">
         <v>500</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="6">
         <v>16.600000000000001</v>
       </c>
-      <c r="C7">
+      <c r="C8" s="6">
         <v>3.16</v>
       </c>
-      <c r="D7">
+      <c r="D8" s="7">
         <f t="shared" si="0"/>
         <v>0.19036144578313252</v>
       </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="4">
+      <c r="E8" s="6">
+        <v>480</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="1"/>
+        <v>93.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3">
         <v>1000</v>
       </c>
-      <c r="B8">
+      <c r="B9" s="6">
         <v>16.600000000000001</v>
       </c>
-      <c r="C8">
+      <c r="C9" s="6">
         <v>6.48</v>
       </c>
-      <c r="D8">
+      <c r="D9" s="7">
         <f t="shared" si="0"/>
         <v>0.39036144578313253</v>
       </c>
-      <c r="E8">
+      <c r="E9" s="6">
         <v>236</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="4">
+      <c r="F9" s="6">
+        <f t="shared" si="1"/>
+        <v>95.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3">
         <v>2000</v>
       </c>
-      <c r="B9">
+      <c r="B10" s="6">
         <v>16.8</v>
       </c>
-      <c r="C9">
+      <c r="C10" s="6">
         <v>12.6</v>
       </c>
-      <c r="D9">
+      <c r="D10" s="7">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="E9">
+      <c r="E10" s="6">
         <v>120</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="4">
+      <c r="F10" s="6">
+        <f t="shared" si="1"/>
+        <v>93.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3">
         <v>5000</v>
       </c>
-      <c r="B10">
+      <c r="B11" s="6">
         <v>12.9</v>
       </c>
-      <c r="C10">
+      <c r="C11" s="6">
         <v>22.6</v>
       </c>
-      <c r="D10">
+      <c r="D11" s="7">
         <f t="shared" si="0"/>
         <v>1.751937984496124</v>
       </c>
-      <c r="E10">
+      <c r="E11" s="6">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="4">
+      <c r="F11" s="6">
+        <f t="shared" si="1"/>
+        <v>100.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3">
         <v>10000</v>
       </c>
-      <c r="B11">
+      <c r="B12" s="6">
         <v>4.72</v>
       </c>
-      <c r="C11">
+      <c r="C12" s="6">
         <v>12.5</v>
       </c>
-      <c r="D11">
+      <c r="D12" s="7">
         <f t="shared" si="0"/>
         <v>2.648305084745763</v>
       </c>
-      <c r="E11">
+      <c r="E12" s="6">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="4">
+      <c r="F12" s="6">
+        <f t="shared" si="1"/>
+        <v>111.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3">
         <v>20000</v>
       </c>
-      <c r="B12">
+      <c r="B13" s="6">
         <v>2.4</v>
       </c>
-      <c r="C12">
+      <c r="C13" s="6">
         <v>17.2</v>
       </c>
-      <c r="D12">
+      <c r="D13" s="7">
         <f t="shared" si="0"/>
         <v>7.166666666666667</v>
       </c>
-      <c r="E12">
+      <c r="E13" s="6">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="4">
+      <c r="F13" s="6">
+        <f t="shared" si="1"/>
+        <v>133.92000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3">
         <v>50000</v>
       </c>
-      <c r="B13">
+      <c r="B14" s="6">
         <f>552/1000</f>
         <v>0.55200000000000005</v>
       </c>
-      <c r="C13">
+      <c r="C14" s="6">
         <v>5.6</v>
       </c>
-      <c r="D13">
+      <c r="D14" s="7">
         <f t="shared" si="0"/>
         <v>10.144927536231883</v>
       </c>
-      <c r="E13">
+      <c r="E14" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="4">
+      <c r="F14" s="6">
+        <f t="shared" si="1"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3">
         <v>100000</v>
       </c>
-      <c r="B14">
+      <c r="B15" s="6">
         <v>0.54800000000000004</v>
       </c>
-      <c r="C14">
+      <c r="C15" s="6">
         <v>3.4</v>
       </c>
-      <c r="D14">
+      <c r="D15" s="7">
         <f t="shared" si="0"/>
         <v>6.2043795620437949</v>
       </c>
-      <c r="E14">
+      <c r="E15" s="6">
         <v>1.56</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="4">
+      <c r="F15" s="6">
+        <f t="shared" si="1"/>
+        <v>123.84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="3">
         <v>200000</v>
       </c>
-      <c r="B15">
+      <c r="B16" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C15">
+      <c r="C16" s="6">
         <v>1.74</v>
       </c>
-      <c r="D15">
+      <c r="D16" s="7">
         <f t="shared" si="0"/>
         <v>3.1071428571428568</v>
       </c>
-      <c r="E15">
+      <c r="E16" s="6">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="4">
+      <c r="F16" s="6">
+        <f t="shared" si="1"/>
+        <v>100.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3">
         <v>500000</v>
       </c>
-      <c r="B16">
+      <c r="B17" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C16">
+      <c r="C17" s="6">
         <f>728/1000</f>
         <v>0.72799999999999998</v>
       </c>
-      <c r="D16">
+      <c r="D17" s="7">
         <f t="shared" si="0"/>
         <v>1.2999999999999998</v>
       </c>
-      <c r="E16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="4">
+      <c r="E17" s="6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="1"/>
+        <v>75.599999999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3">
         <v>1000000</v>
       </c>
-      <c r="B17">
+      <c r="B18" s="6">
         <v>0.49199999999999999</v>
       </c>
-      <c r="C17">
+      <c r="C18" s="6">
         <f>352/1000</f>
         <v>0.35199999999999998</v>
       </c>
-      <c r="D17">
+      <c r="D18" s="7">
         <f t="shared" si="0"/>
         <v>0.71544715447154472</v>
       </c>
-      <c r="E17">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="5">
+      <c r="E18" s="6">
+        <v>0.13</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="1"/>
+        <v>133.19999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="5">
         <v>2000000</v>
       </c>
-      <c r="B18">
+      <c r="B19" s="6">
         <f>468/1000</f>
         <v>0.46800000000000003</v>
       </c>
-      <c r="C18">
+      <c r="C19" s="6">
         <f>160/1000</f>
         <v>0.16</v>
       </c>
-      <c r="D18">
+      <c r="D19" s="7">
         <f t="shared" si="0"/>
         <v>0.34188034188034189</v>
       </c>
-      <c r="E18">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="4">
+      <c r="E19" s="6">
+        <v>0.254</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="1"/>
+        <v>-2.8799999999999955</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3">
         <v>3000000</v>
       </c>
-      <c r="B19">
+      <c r="B20" s="6">
         <v>0.33600000000000002</v>
       </c>
-      <c r="C19">
+      <c r="C20" s="6">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="D19">
+      <c r="D20" s="7">
         <f t="shared" si="0"/>
         <v>0.17559523809523808</v>
       </c>
-      <c r="E19">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="5"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="C22">
-        <f>2.6</f>
-        <v>2.6</v>
+      <c r="E20" s="6">
+        <v>0.13</v>
+      </c>
+      <c r="F20" s="6">
+        <f t="shared" si="1"/>
+        <v>39.599999999999994</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
wykresy + poprawa fazy
</commit_message>
<xml_diff>
--- a/Pomiary_lab2.xlsx
+++ b/Pomiary_lab2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580"/>
@@ -11,7 +11,7 @@
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -60,11 +60,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +102,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -138,20 +147,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -160,18 +163,44 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -194,20 +223,30 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16448722402346763"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="stacked"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$A$3:$A$20</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
@@ -265,8 +304,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Arkusz1!$D$3:$D$20</c:f>
               <c:numCache>
@@ -328,20 +367,30 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:hiLowLines/>
-        <c:marker val="1"/>
-        <c:axId val="95093888"/>
-        <c:axId val="95095808"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="95093888"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="192723120"/>
+        <c:axId val="191965760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="192723120"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -364,10 +413,12 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -375,20 +426,20 @@
             <a:pPr>
               <a:defRPr sz="1000"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95095808"/>
+        <c:crossAx val="191965760"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="95095808"/>
+        <c:axId val="191965760"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -409,15 +460,20 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95093888"/>
+        <c:crossAx val="192723120"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -429,7 +485,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -453,19 +519,32 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="stacked"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16154392465647677"/>
+          <c:y val="0.15847659667541558"/>
+          <c:w val="0.74878937007874014"/>
+          <c:h val="0.68387685914260721"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Arkusz1!$A$3:$A$20</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
@@ -523,83 +602,93 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Arkusz1!$F$3:$F$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>118.8</c:v>
+                  <c:v>-118.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110.88</c:v>
+                  <c:v>-110.88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>97.2</c:v>
+                  <c:v>-97.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>95.04</c:v>
+                  <c:v>-95.04</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95.04</c:v>
+                  <c:v>-95.04</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>93.6</c:v>
+                  <c:v>-93.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>95.04</c:v>
+                  <c:v>-95.04</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>93.6</c:v>
+                  <c:v>-93.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100.8</c:v>
+                  <c:v>-100.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>111.6</c:v>
+                  <c:v>-111.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>133.92000000000002</c:v>
+                  <c:v>-133.92000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>162</c:v>
+                  <c:v>-162</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>123.84</c:v>
+                  <c:v>-123.84</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>100.8</c:v>
+                  <c:v>-100.8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>75.599999999999994</c:v>
+                  <c:v>-75.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>133.19999999999999</c:v>
+                  <c:v>-133.19999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-2.8799999999999955</c:v>
+                  <c:v>2.8799999999999955</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>39.599999999999994</c:v>
+                  <c:v>-39.599999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:hiLowLines/>
-        <c:marker val="1"/>
-        <c:axId val="92532096"/>
-        <c:axId val="107285504"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="92532096"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="195198704"/>
+        <c:axId val="191968560"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="195198704"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -622,21 +711,22 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107285504"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="191968560"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="107285504"/>
+        <c:axId val="191968560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -668,15 +758,20 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92532096"/>
+        <c:crossAx val="195198704"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -690,16 +785,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -720,15 +815,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -794,7 +889,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -826,9 +921,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -860,6 +956,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -1035,23 +1132,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15.75">
+    <row r="2" spans="1:19" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1064,413 +1161,456 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3">
+      <c r="S2" s="10"/>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="7">
         <v>10</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="4">
         <v>12.4</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <f>16/1000</f>
         <v>1.6E-2</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <f>C3/B3</f>
         <v>1.2903225806451613E-3</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>17000</v>
       </c>
-      <c r="F3" s="6">
-        <f>180-((A3*360*E3)/1000000)</f>
-        <v>118.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3">
+      <c r="F3" s="4">
+        <f>-180+((A3*360*E3)/1000000)</f>
+        <v>-118.8</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="S3" s="9"/>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="7">
         <v>20</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="4">
         <v>16</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>0.14799999999999999</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <f t="shared" ref="D4:D20" si="0">C4/B4</f>
         <v>9.2499999999999995E-3</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>9600</v>
       </c>
-      <c r="F4" s="6">
-        <f t="shared" ref="F4:F20" si="1">180-((A4*360*E4)/1000000)</f>
-        <v>110.88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3">
+      <c r="F4" s="4">
+        <f t="shared" ref="F4:F20" si="1">-180+((A4*360*E4)/1000000)</f>
+        <v>-110.88</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="S4" s="9"/>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="7">
         <v>50</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>16.600000000000001</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>0.32</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <f t="shared" si="0"/>
         <v>1.9277108433734938E-2</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>4600</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="4">
         <f t="shared" si="1"/>
-        <v>97.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3">
+        <v>-97.2</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="S5" s="9"/>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="7">
         <v>100</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>16.600000000000001</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>0.63</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <f t="shared" si="0"/>
         <v>3.7951807228915661E-2</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>2360</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="4">
         <f t="shared" si="1"/>
-        <v>95.04</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="3">
+        <v>-95.04</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="S6" s="9"/>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="7">
         <v>200</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>16.600000000000001</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <v>1.24</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <f t="shared" si="0"/>
         <v>7.4698795180722879E-2</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>1180</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="4">
         <f t="shared" si="1"/>
-        <v>95.04</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="3">
+        <v>-95.04</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="S7" s="9"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="7">
         <v>500</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <v>16.600000000000001</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>3.16</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <f t="shared" si="0"/>
         <v>0.19036144578313252</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="4">
         <v>480</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="4">
         <f t="shared" si="1"/>
-        <v>93.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="3">
+        <v>-93.6</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="S8" s="9"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="7">
         <v>1000</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>16.600000000000001</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>6.48</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <f t="shared" si="0"/>
         <v>0.39036144578313253</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="4">
         <v>236</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="4">
         <f t="shared" si="1"/>
-        <v>95.04</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="3">
+        <v>-95.04</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="S9" s="9"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="7">
         <v>2000</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>16.8</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <v>12.6</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="4">
         <v>120</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="4">
         <f t="shared" si="1"/>
-        <v>93.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="3">
+        <v>-93.6</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="S10" s="9"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="7">
         <v>5000</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>12.9</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <v>22.6</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <f t="shared" si="0"/>
         <v>1.751937984496124</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="4">
         <v>44</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="4">
         <f t="shared" si="1"/>
-        <v>100.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="3">
+        <v>-100.8</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="S11" s="9"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="7">
         <v>10000</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>4.72</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>12.5</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <f t="shared" si="0"/>
         <v>2.648305084745763</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <v>19</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="4">
         <f t="shared" si="1"/>
-        <v>111.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="3">
+        <v>-111.6</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="S12" s="9"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="7">
         <v>20000</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <v>2.4</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <v>17.2</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <f t="shared" si="0"/>
         <v>7.166666666666667</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="4">
         <v>6.4</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="4">
         <f t="shared" si="1"/>
-        <v>133.92000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="3">
+        <v>-133.92000000000002</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="S13" s="9"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="7">
         <v>50000</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <f>552/1000</f>
         <v>0.55200000000000005</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <v>5.6</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <f t="shared" si="0"/>
         <v>10.144927536231883</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="4">
         <v>1</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="4">
         <f t="shared" si="1"/>
-        <v>162</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="3">
+        <v>-162</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="S14" s="9"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="7">
         <v>100000</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <v>0.54800000000000004</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="4">
         <v>3.4</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="5">
         <f t="shared" si="0"/>
         <v>6.2043795620437949</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="4">
         <v>1.56</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="4">
         <f t="shared" si="1"/>
-        <v>123.84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="3">
+        <v>-123.84</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="S15" s="9"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="7">
         <v>200000</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="4">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="4">
         <v>1.74</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="5">
         <f t="shared" si="0"/>
         <v>3.1071428571428568</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
-        <v>100.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="3">
+        <v>-100.8</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="S16" s="9"/>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17" s="7">
         <v>500000</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="4">
         <f>728/1000</f>
         <v>0.72799999999999998</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <f t="shared" si="0"/>
         <v>1.2999999999999998</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="4">
         <v>0.57999999999999996</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="4">
         <f t="shared" si="1"/>
-        <v>75.599999999999994</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="3">
+        <v>-75.599999999999994</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="S17" s="9"/>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" s="7">
         <v>1000000</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <v>0.49199999999999999</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="4">
         <f>352/1000</f>
         <v>0.35199999999999998</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="5">
         <f t="shared" si="0"/>
         <v>0.71544715447154472</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="4">
         <v>0.13</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="4">
         <f t="shared" si="1"/>
-        <v>133.19999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="5">
+        <v>-133.19999999999999</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="S18" s="9"/>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" s="8">
         <v>2000000</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <f>468/1000</f>
         <v>0.46800000000000003</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="4">
         <f>160/1000</f>
         <v>0.16</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="5">
         <f t="shared" si="0"/>
         <v>0.34188034188034189</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="4">
         <v>0.254</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="4">
         <f t="shared" si="1"/>
-        <v>-2.8799999999999955</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="3">
+        <v>2.8799999999999955</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="S19" s="9"/>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" s="7">
         <v>3000000</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <v>0.33600000000000002</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="4">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="5">
         <f t="shared" si="0"/>
         <v>0.17559523809523808</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="4">
         <v>0.13</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="4">
         <f t="shared" si="1"/>
-        <v>39.599999999999994</v>
+        <v>-39.599999999999994</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="S20" s="9"/>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="C23">
+        <f>1000000</f>
+        <v>1000000</v>
       </c>
     </row>
   </sheetData>
@@ -1481,7 +1621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1494,7 +1634,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>